<commit_message>
added submission and submission zip
</commit_message>
<xml_diff>
--- a/src/DataAlgoGraph.xlsx
+++ b/src/DataAlgoGraph.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jayanthprathipati/Development/4104_proj/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="15315" windowHeight="8505"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="15320" windowHeight="8500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -32,7 +42,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>n   (</t>
+      <t>n  (line sweep)  (</t>
     </r>
     <r>
       <rPr>
@@ -57,7 +67,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">b   </t>
+      <t xml:space="preserve">b (brute force)   </t>
     </r>
     <r>
       <rPr>
@@ -176,7 +186,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tn   (milliseconds)</c:v>
+                  <c:v>Tn  (line sweep)  (milliseconds)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -188,25 +198,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -218,25 +228,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>146.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,25 +266,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -286,25 +296,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1445</c:v>
+                  <c:v>1506.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5550</c:v>
+                  <c:v>3209.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -319,11 +329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53129984"/>
-        <c:axId val="53115520"/>
+        <c:axId val="-2128669136"/>
+        <c:axId val="-2128736352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53129984"/>
+        <c:axId val="-2128669136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,12 +367,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53115520"/>
+        <c:crossAx val="-2128736352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53115520"/>
+        <c:axId val="-2128736352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53129984"/>
+        <c:crossAx val="-2128669136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -419,15 +429,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -492,7 +502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,7 +537,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -739,17 +749,17 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -771,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
@@ -782,7 +792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>500</v>
       </c>
@@ -790,51 +800,51 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1000</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2000</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10000</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>1445</v>
+        <v>1506</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20000</v>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="C8">
-        <v>5550</v>
+        <v>3209</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +860,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -862,7 +872,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>